<commit_message>
Revert to last commit before v4
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Commands" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">Commands!$C$132</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">Commands!$C$133</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="408">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -1003,6 +1003,12 @@
   </si>
   <si>
     <t xml:space="preserve">sets the PID target set value SV given in C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidSVbuttons(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggles the visibility of the PID SV buttons</t>
   </si>
   <si>
     <t xml:space="preserve">pidRS(&lt;rs&gt;)</t>
@@ -2176,10 +2182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C167"/>
+  <dimension ref="A1:C168"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C132" activeCellId="0" sqref="C132"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B104" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C113" activeCellId="0" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3183,15 +3189,15 @@
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>133</v>
+        <v>329</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
-        <v>330</v>
+        <v>133</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>331</v>
@@ -3199,18 +3205,18 @@
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>137</v>
+        <v>332</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>138</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="3" t="s">
-        <v>332</v>
+        <v>137</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>333</v>
+        <v>138</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3366,17 +3372,17 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="s">
+      <c r="B146" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="B146" s="3" t="s">
+      <c r="C146" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C146" s="1" t="s">
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
         <v>375</v>
       </c>
@@ -3434,15 +3440,15 @@
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="3" t="s">
-        <v>240</v>
+        <v>389</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="3" t="s">
-        <v>390</v>
+        <v>240</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>391</v>
@@ -3458,26 +3464,26 @@
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B158" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>387</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="B159" s="3" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>398</v>
@@ -3485,69 +3491,77 @@
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="3" t="s">
-        <v>377</v>
+        <v>399</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="B161" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B162" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="C162" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B162" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="3" t="s">
-        <v>131</v>
+        <v>403</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>132</v>
+        <v>404</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>403</v>
+        <v>134</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>138</v>
+        <v>405</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="3" t="s">
-        <v>404</v>
+        <v>137</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>405</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B168" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>